<commit_message>
Update doc SIHAM (cf. mail de Maura Santoro de Montpellier)
</commit_message>
<xml_diff>
--- a/doc/Connecteurs-Import/Siham/Partie_A_SIHAM_REF/A_V15_SIHAM_REF_Suivi_deploiement_MPD_OSE.xlsx
+++ b/doc/Connecteurs-Import/Siham/Partie_A_SIHAM_REF/A_V15_SIHAM_REF_Suivi_deploiement_MPD_OSE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10275"/>
   </bookViews>
   <sheets>
     <sheet name="A_SIHAM_REF_MPD_OSE_2020" sheetId="8" r:id="rId1"/>
@@ -158,11 +158,6 @@
     <t>v2.2 : 03/12/2020 : V15 UM_SYNCHRO_VOIRIE + UM_ALIM_ ADRESSE_NUMERO_COMPL</t>
   </si>
   <si>
-    <t xml:space="preserve">1ere fois : A_1_T_OSE_create_table_v2.0_utf8.sql
-Montée de version : A_1_T_OSE_alter_tables_v2.0.sql
-</t>
-  </si>
-  <si>
     <t>v2.0 : 30/11 au 02/02/21 : UM_VOIRIE + UM_PARAM_ETABL</t>
   </si>
   <si>
@@ -194,12 +189,61 @@
   <si>
     <t>Code couleurs :</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1ere fois : A_1_T_OSE_create_table_v2.0_utf8.sql
+  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">!! Montée de version précédente : 
+          - Si déjà en Connecteur_SIHAM_OSE_v1.1_2019-12 : A_1_T_OSE_alter_tables_v2.0.sql
+          - Si en Connecteur_SIHAM_OSE_v1.0_2019-05 ou 2019-02 : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>01_T_OSE_alter_tables_v1.4_a_v1.8.sql</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> puis A_1_T_OSE_alter_tables_v2.0.sql</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,6 +304,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -627,6 +686,43 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -648,43 +744,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1003,7 +1062,7 @@
   <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C7" sqref="C7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,27 +1078,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2" s="16"/>
       <c r="F2" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="17"/>
-      <c r="F3" s="57" t="s">
-        <v>39</v>
+      <c r="F3" s="40" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -1060,44 +1119,44 @@
       </c>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="55" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
     </row>
     <row r="6" spans="1:27" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="5"/>
       <c r="C6" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="O6" s="7"/>
       <c r="AA6" s="9"/>
     </row>
-    <row r="7" spans="1:27" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
+    <row r="7" spans="1:27" s="1" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="56"/>
       <c r="B7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
+      <c r="C7" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
       <c r="O7" s="7"/>
       <c r="AA7" s="9"/>
     </row>
     <row r="8" spans="1:27" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="5"/>
       <c r="C8" s="28" t="s">
         <v>14</v>
@@ -1108,17 +1167,17 @@
       <c r="AA8" s="9"/>
     </row>
     <row r="9" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="5"/>
       <c r="C9" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="5"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -1126,7 +1185,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="5"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -1134,49 +1193,49 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="C12" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="24"/>
       <c r="C13" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="24"/>
       <c r="C14" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="56"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="18"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="24"/>
       <c r="C15" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
+        <v>33</v>
+      </c>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="5"/>
       <c r="C16" s="11"/>
       <c r="D16" s="12"/>
@@ -1184,29 +1243,29 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="C17" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
+      <c r="A18" s="56"/>
       <c r="B18" s="5"/>
       <c r="C18" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
+      <c r="A19" s="56"/>
       <c r="B19" s="5"/>
       <c r="C19" s="19" t="s">
         <v>16</v>
@@ -1216,7 +1275,7 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
+      <c r="A20" s="56"/>
       <c r="B20" s="5"/>
       <c r="C20" s="19" t="s">
         <v>30</v>
@@ -1226,7 +1285,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="44"/>
+      <c r="A21" s="57"/>
       <c r="B21" s="5"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
@@ -1234,7 +1293,7 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="46" t="s">
         <v>26</v>
       </c>
       <c r="B22" s="33"/>
@@ -1246,19 +1305,19 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="53"/>
-      <c r="E23" s="54"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="50"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="5"/>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -1266,41 +1325,41 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="53"/>
-      <c r="E25" s="54"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="50"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="5"/>
       <c r="C26" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="50"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="52" t="s">
+      <c r="C27" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="53"/>
-      <c r="E27" s="54"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="50"/>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="51"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
@@ -1308,7 +1367,7 @@
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="41" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="33"/>
@@ -1320,17 +1379,17 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="45"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="47"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="49"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="45"/>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="45"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="5"/>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
@@ -1338,19 +1397,19 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="45"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="48"/>
-      <c r="E32" s="49"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="45"/>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="46"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="21"/>
       <c r="C33" s="22" t="s">
         <v>25</v>
@@ -1395,6 +1454,12 @@
   </sheetData>
   <autoFilter ref="A4:E47"/>
   <mergeCells count="13">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A5:A21"/>
+    <mergeCell ref="C17:E17"/>
     <mergeCell ref="A29:A33"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C32:E32"/>
@@ -1402,12 +1467,6 @@
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C27:E27"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A5:A21"/>
-    <mergeCell ref="C17:E17"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="91" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Connecteur Siham import V18
</commit_message>
<xml_diff>
--- a/doc/Connecteurs-Import/Siham/Partie_A_SIHAM_REF/A_V15_SIHAM_REF_Suivi_deploiement_MPD_OSE.xlsx
+++ b/doc/Connecteurs-Import/Siham/Partie_A_SIHAM_REF/A_V15_SIHAM_REF_Suivi_deploiement_MPD_OSE.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="A_SIHAM_REF_MPD_OSE" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">A_SIHAM_REF_MPD_OSE!$A$4:$E$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">A_SIHAM_REF_MPD_OSE!$A$4:$E$47</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Etapes</t>
   </si>
@@ -58,18 +58,6 @@
   </si>
   <si>
     <t>automatisation (si besoin) : lance_synchro_Siham_vers_OseProse.sh</t>
-  </si>
-  <si>
-    <t>v2.0 : 15/11/2019 : renommage prose_annee_id</t>
-  </si>
-  <si>
-    <t>v1.8 : 02/12/2019 : UM_STRUCTURE renommage tem_manu en eotp_DU_defaut + eotp_DN_defaut</t>
-  </si>
-  <si>
-    <t>v2.1 : 07/07/20 : mapping statut v12</t>
-  </si>
-  <si>
-    <t>v2.1 : 03/07/20 : substr ll_grade</t>
   </si>
   <si>
     <t>A_recompiler_fonction_proc.sql</t>
@@ -155,16 +143,7 @@
     </r>
   </si>
   <si>
-    <t>v2.2 : 03/12/2020 : V15 UM_SYNCHRO_VOIRIE + UM_ALIM_ ADRESSE_NUMERO_COMPL</t>
-  </si>
-  <si>
-    <t>v2.0 : 30/11 au 02/02/21 : UM_VOIRIE + UM_PARAM_ETABL</t>
-  </si>
-  <si>
     <t>A_2_F_OSE_function_v2.2.sql</t>
-  </si>
-  <si>
-    <t>v2.2 : 03/12/2020 : V15 nouvelles  fonctions  + adaptations</t>
   </si>
   <si>
     <t>A_3_P_OSE_procedure_insert_tables_src_v2.2.sql</t>
@@ -181,14 +160,32 @@
 DBLINK BI : nommé @BI  (vers Base intermédiaire LDAP - sera utile plus tard pour partie B)</t>
   </si>
   <si>
-    <t>Déjà inclus dans la livraison CAEN 12/2019</t>
-  </si>
-  <si>
     <t>Code couleurs :</t>
   </si>
   <si>
+    <t>Modifications pour OSE V15 connecteur v2.1</t>
+  </si>
+  <si>
+    <t>v2.1 : 28/05/21 MYP modifs taille champs adr</t>
+  </si>
+  <si>
+    <t>v2.3 : 28/05/21 MYP modifs taille champs adr</t>
+  </si>
+  <si>
+    <t>v2.4 : 11/06/21 : raz numero_compl_code si inexistant dans OSE.ADRESSE_NUMERO_COMPL</t>
+  </si>
+  <si>
+    <t>v2.5 : 18/10/21 : correction synchro adr_numero_compl</t>
+  </si>
+  <si>
+    <t>v2.3 : ajout UM_AFFICH_UO_INF (ne concerne que Prose)</t>
+  </si>
+  <si>
+    <t>v2.5b : 04/02/22 : ajout .world au dblink</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">1ere fois : A_1_T_OSE_create_table_v2.0_utf8.sql
+      <t xml:space="preserve">1ere fois : A_1_T_OSE_create_table_utf8.sql
   </t>
     </r>
     <r>
@@ -236,26 +233,23 @@
     </r>
   </si>
   <si>
-    <t>Modifications pour OSE V15 connecteur v2.0</t>
-  </si>
-  <si>
-    <t>Modifications pour OSE V15 connecteur v2.1</t>
-  </si>
-  <si>
-    <t>v2.1 : 28/05/21 MYP modifs taille champs adr</t>
-  </si>
-  <si>
-    <t>v2.3 : 28/05/21 MYP modifs taille champs adr</t>
-  </si>
-  <si>
-    <t>v2.4 : 11/06/21 : raz numero_compl_code si inexistant dans OSE.ADRESSE_NUMERO_COMPL</t>
+    <t>v2.1 : 28/05/21 MYP modifs taille champs adr (relivré pas de modif depuis la v2.1)</t>
+  </si>
+  <si>
+    <t>v2.3b : 04/02/22 : ajout .world au dblink</t>
+  </si>
+  <si>
+    <t>Modifications pour OSE V18 connecteur v3.0 du 20/07/22</t>
+  </si>
+  <si>
+    <t>v2.2 : 20/07/22 param C_ORG_RATTACH en multi uai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,13 +267,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -332,24 +319,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -387,6 +362,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -597,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -629,9 +610,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -647,9 +625,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -665,108 +640,99 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1084,10 +1050,10 @@
     <tabColor theme="2" tint="-0.499984740745262"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA53"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,117 +1064,115 @@
     <col min="4" max="4" width="43" style="2" customWidth="1"/>
     <col min="5" max="5" width="42.140625" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="41.140625" customWidth="1"/>
+    <col min="7" max="7" width="51.7109375" customWidth="1"/>
     <col min="15" max="15" width="9.140625" style="6"/>
     <col min="27" max="27" width="41.140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B2" s="15"/>
+      <c r="G2" s="31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="16"/>
+      <c r="G3" s="35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:27" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="54"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="G1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="16"/>
-      <c r="G2" s="26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="17"/>
-      <c r="G3" s="40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-    </row>
-    <row r="6" spans="1:27" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
       <c r="O6" s="7"/>
       <c r="AA6" s="9"/>
     </row>
     <row r="7" spans="1:27" s="1" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
-      <c r="B7" s="29" t="s">
+      <c r="A7" s="54"/>
+      <c r="B7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
+      <c r="C7" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="O7" s="7"/>
       <c r="AA7" s="9"/>
     </row>
-    <row r="8" spans="1:27" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
+    <row r="8" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="54"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="12"/>
+      <c r="C8" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="11"/>
       <c r="E8" s="12"/>
-      <c r="O8" s="7"/>
-      <c r="AA8" s="9"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="59"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="13" t="s">
-        <v>31</v>
+      <c r="C9" s="38" t="s">
+        <v>39</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="59"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="38" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="11"/>
@@ -1216,7 +1180,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="5"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -1224,249 +1188,235 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
-      <c r="B12" s="29" t="s">
+      <c r="A12" s="54"/>
+      <c r="B12" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
+      <c r="C12" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="59"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="18"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="36" t="s">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="54"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="54"/>
+      <c r="B16" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="54"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="59"/>
-      <c r="B17" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="57" t="s">
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="54"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="54"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="11"/>
+      <c r="C19" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="54"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="19" t="s">
-        <v>30</v>
+      <c r="C20" s="34" t="s">
+        <v>37</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="59"/>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="55"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="43" t="s">
-        <v>43</v>
-      </c>
+      <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="C22" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="60"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="44"/>
+      <c r="B23" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="47"/>
+      <c r="E23" s="48"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
+      <c r="A24" s="44"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="34" t="s">
+      <c r="A25" s="44"/>
+      <c r="B25" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="47"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A26" s="44"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="44"/>
+      <c r="B27" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="47"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="45"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="39"/>
+      <c r="B30" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="41"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="39"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="39"/>
+      <c r="B32" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="52"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
-      <c r="B27" s="34" t="s">
+      <c r="C32" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="51" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="52"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A28" s="49"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="49"/>
-      <c r="B29" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="51" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="52"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="50"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
-      <c r="B32" s="35" t="s">
+      <c r="D32" s="42"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="40"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
-      <c r="B34" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="47"/>
-      <c r="E34" s="48"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="45"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="23"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1481,43 +1431,37 @@
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F45" s="1"/>
-    </row>
-    <row r="53" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P53" s="10"/>
+    <row r="51" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P51" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:E49"/>
+  <autoFilter ref="A4:E47"/>
   <mergeCells count="13">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C12:E12"/>
-    <mergeCell ref="A5:A23"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A5:A21"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="C30:E30"/>
     <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="C23:E23"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C29:E29"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="91" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>